<commit_message>
Changes to add extract and LLM summarize with manual testing documentation. The results are also documented
</commit_message>
<xml_diff>
--- a/manual_testing/Question_Answers_GastroAssist.xlsx
+++ b/manual_testing/Question_Answers_GastroAssist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avssm\fullstack-projects\gastroassist\manual_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79436E2-D8BF-45F0-B606-98A4D266B7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658E609A-A37D-4562-9A95-925FCDE50971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9257E51F-A0A0-4460-844C-C8606EB65798}"/>
   </bookViews>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D541741E-0F0F-4164-99D4-6E8DAD031701}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Documentation details updated  and batch testing with LLM as a judge and metrics related to it.
</commit_message>
<xml_diff>
--- a/manual_testing/Question_Answers_GastroAssist.xlsx
+++ b/manual_testing/Question_Answers_GastroAssist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avssm\fullstack-projects\gastroassist\manual_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658E609A-A37D-4562-9A95-925FCDE50971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FB2F6D-F963-442A-860A-BA9BA8451C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9257E51F-A0A0-4460-844C-C8606EB65798}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Expected Answer</t>
   </si>
@@ -59,102 +59,45 @@
     <t>H. pylori damages the gastric mucosa by producing urease, which creates a local alkaline environment, allowing the bacteria to colonize and trigger inflammation and ulceration.</t>
   </si>
   <si>
-    <t>Based on the information I found:
-The pathophysiology of peptic ulcer disease (PUD) is often described as an imbalance between aggressive factors such as acid and pepsin and alterations in the mucosal protective mechanisms. Helicobacter pylori is a gram-negative organism that has been identified as a potential causative agent in the pathogenesis of PUD.
-Helicobacter pylori infection of gastric mucosa is widespread, causing asymptomatic superficial gastritis; however, symptomatic disease in the form of duodenal and gastric ulcers is present only in a small proportion of infected individuals.H pylori causes most of the peptic ulcer disease that is not associated with nonsteroidal anti-inflammatory drug use or gastrinoma.
-Peptic ulcers are frequently encountered in the primary care setting and understanding associated risk factors is key to disease prevention and management. Definition and Epidemiology Peptic ulcers are acid-induced lesions found in the stomach and duodenum characterized by denuded mucosa with the defect extending into the submucosa or muscularis propria. 1 Lesions that do not reach this depth ...
-The pathophysiology of peptic ulcer disease (PUD) is often described as an imbalance between aggressive factors such as acid and pepsin and alterations in the mucosal protective mechanisms. Helicobacter pylori is a gram-negative organism that has been identified as a potential causative agent in the …</t>
-  </si>
-  <si>
-    <t>Based on the information I found:
-Epigastric abdominal pain that improves with meals is the hallmark of PUD. However, in some cases, symptoms of PUD may worsen with meals. NSAID use is associated with the development of PUD. Hematemesis, if present, suggests more complicated disease including bleeding ulcer and warrants urgent GI referral and endoscopy.
-It has many causes, including overeating, lactose intolerance, and underlying conditions like gastroesophageal reflux disease (GERD), inflammation, and infection. Heartburn is a symptom of acid reflux and GERD, commonly described as a burning feeling in your chest after you eat. However, they may lead to acid reflux or GERD, which can cause epigastric pain or heartburn. This condition may result from acid reflux, which can cause epigastric pain. If an underlying condition such as GERD, Barrett’s esophagus, or peptic ulcer disease is causing your epigastric pain, you’ll likely require acid-blocking medications. Symptoms of Acid RefluxLearn more about acid reflux, a condition that occurs when stomach acids back up into the esophagus through the lower esophageal sphincter.
-The classic symptom is burning epigastric pain after meals. Pain that occurs immediately after meals is a classic symptom of gastric ulcer. Pain that occurs 2 to 3 hours after meals and that is relieved by food or antacids is a strong indicator of duodenal ulcer. 13 Other symptoms include dyspepsia, bloating, distention, heartburn, and chest ...
-Epigastric abdominal pain that improves with meals is the hallmark of PUD. However, in some cases, symptoms of PUD may worsen with meals. NSAID use is associated with the development of PUD. Hematemesis, if present, suggests more complicated disease including bleeding ulcer and warrants urgent GI referral and endoscopy.</t>
-  </si>
-  <si>
     <t>What are the red flag symptoms in a patient with dyspepsia that warrant urgent endoscopy?</t>
   </si>
   <si>
     <t>Red flags include unintentional weight loss, persistent vomiting, dysphagia, gastrointestinal bleeding, and anemia.</t>
   </si>
   <si>
-    <t>Based on the information I found:
-What are the high-risk groups or red flags that should never be ignored in patients with dyspepsia? Paul Moayyedi: Our data would suggest red flags are not as important as the textbooks would suggest. Most patients with the so-called red flags—that should be things like weight loss, anemia, dysphagia, vomiting—do not have organic pathology.
-Flow Diagram: DYSPEPSIA Diagnosis and Management - Expanded Detail. 1. Establish the diagnosis of dyspepsia as defined above through history and physical examination, excluding worrisome features or red flags. In the presence of any red flags, referral to Gastroenterology for consideration of urgent endoscopic investigation is recommended, even
-What are the high-risk groups or red flags that should never be ignored in patients with dyspepsia? Paul Moayyedi: Our data would suggest red flags are not as important as the textbooks would suggest. Most patients with the so-called red flags—that should be things like weight loss, anemia, dysphagia, vomiting—do not have organic pathology.
-Red flags are signs and symptoms found in the patient's history and clinical examination. ... red eye and dyspepsia as well. Identification of red flags warrant investigations and or referral and is an integral part of primary care and of immense value to primary care doctors. ... Red flags in patients presenting with headache: Clinical ...</t>
-  </si>
-  <si>
     <t xml:space="preserve"> In a patient with elevated liver enzymes, how would you differentiate between hepatocellular and cholestatic injury?</t>
   </si>
   <si>
     <t>Hepatocellular injury shows elevated ALT/AST, while cholestatic injury shows elevated ALP and GGT. The ALT:ALP ratio helps in differentiation.</t>
   </si>
   <si>
-    <t>Based on the information I found:
-Figure re-drawn from BioRender. 1) Hepatocellular pattern: The degree of AST and ALT elevation varies based on the underlying cause of hepatocellular injury.Additionally, the AST/ALT ratio provides diagnostic clues; in alcohol associated liver disease, around 90% of patients have an AST/ALT ratio &gt;2, likely due to alcohol-related depletion of pyridoxal phosphate, needed for ALT synthesis, and ...
-Fig. 2: Serum aminotransferase levels in various liver diseases. Patients with acute viral or ischemic or toxic liver injury reach the highest aminotransferase levels, but there is a broad overlap in aminotransferase values between patients with acute alcoholic hepatitis and autoimmune hepatitis as well as between patients with chronic hepatitis and liver cirrhosis.</t>
-  </si>
-  <si>
     <t>What is the first-line treatment for mild to moderate ulcerative colitis?</t>
   </si>
   <si>
     <t>Aminosalicylates (e.g., mesalamine) administered orally or rectally depending on disease extent.</t>
   </si>
   <si>
-    <t>Based on the information I found:
-An algorithm for the medial management of mild, moderate, and severe ulcerative colitis. Progression along arrows is indicated if prior therapies fail. For mild to moderate disease the first-line therapy is 5-ASA agents. If this is ineffective, steroids can be used to induce remission.
-Ulcerative colitis is a relapsing and remitting disease that is increasing in incidence and prevalence. Management aims to achieve rapid resolution of symptoms, mucosal healing and improvement in a patient's quality of life. 5-aminosalicylate acid medications remain the first-line treatment for mild to moderate disease.
-On MyCrohnsAndColitisTeam, more than 182,000 members come together to ask questions, give advice, and share their stories with others who understand life with ulcerative colitis. What was your first-line treatment for ulcerative colitis? Share your experience in the comments below, or start a conversation by posting on your Activities page.
-Changes to Make to Your Diet To Help With UC. Eating a healthy and well-balanced diet is important even for mild cases of ulcerative colitis. This could help prevent it from getting worse.</t>
-  </si>
-  <si>
     <t>How do you interpret a positive anti-tissue transglutaminase (tTG) IgA test in a symptomatic adult?</t>
   </si>
   <si>
     <t>It strongly suggests celiac disease, but diagnosis should be confirmed with a duodenal biopsy showing villous atrophy while the patient is on a gluten-containing diet.</t>
   </si>
   <si>
-    <t>Based on the information I found:
-Here's how you can interpret these test results: Anti-TTG IgA Test: Negative Result (Below the Reference Range): If your Anti-TTG IgA test result falls below the established reference range (typically less than 4 U/mL or IU/mL), it is usually considered negative or normal. A negative result suggests a low likelihood of celiac disease.
-Positive Test Result. A positive tTG IgA blood test result means that the immune system has produced antibodies against tissue transglutaminase, suggesting an immune response to gluten. This strongly indicates the presence of celiac disease. However, a positive result is typically followed by an intestinal biopsy to confirm the diagnosis.
-The EMA-IgA test has a sensitivity of 86-100% and a specificity of 97-100%. It is less preferred to tTG-IgA because it is more expensive and time-consuming. Additionally, the EMA-IgA results are qualitative rather than quantitative, making them more subjective than tTG-IgA results. Healthcare providers often reserve this test as a follow-up to ...
-Here's how you can interpret these test results: Anti-TTG IgA Test: Negative Result (Below the Reference Range): If your Anti-TTG IgA test result falls below the established reference range (typically less than 4 U/mL or IU/mL), it is usually considered negative or normal. A negative result suggests a low likelihood of celiac disease.</t>
-  </si>
-  <si>
     <t>When is colonoscopy recommended in patients with irritable bowel syndrome (IBS)?</t>
   </si>
   <si>
     <t>Colonoscopy is indicated if there are alarm features like bleeding, anemia, weight loss, family history of colorectal cancer, or age over 50 with new symptoms.</t>
   </si>
   <si>
-    <t>Based on the information I found:
-A colonoscopy isn't a test that can diagnose irritable bowel syndrome (IBS). However, some people with IBS may have this test in order to look for digestive conditions other than IBS. ... A colonoscopy is not used for routine monitoring of IBS. A colonoscopy might be recommended if there are changes to the severity or frequency of symptoms or
-A healthcare professional is likely to start with a complete medical history, physical exam and tests to rule out other conditions, such as celiac disease and inflammatory bowel disease (IBD). These criteria include belly pain and discomfort averaging at least one day a week in the last three months. This also usually occurs with at least two of the following: pain and discomfort related to defecation, a change in the frequency of defecation, or a change in stool consistency. Care at Mayo Clinic Our caring team of Mayo Clinic experts can help you with your irritable bowel syndrome-related health concerns Start Here More Information Irritable bowel syndrome care at Mayo Clinic Colonoscopy CT scan Flexible sigmoidoscopy Show more related information Treatment Treatment of IBS focuses on relieving symptoms so that you can live as symptom-free as possible.
-Diagnostic yield of colonoscopy for organic disease in irritable bowel syndrome and its risk factors: A meta-analysis. https://pubmed.ncbi.nlm.nih.gov/36168183/ Yang Q, et al. (2022).
-A colonoscopy isn't a test that can diagnose irritable bowel syndrome (IBS). However, some people with IBS may have this test in order to look for digestive conditions other than IBS. ... A colonoscopy is not used for routine monitoring of IBS. A colonoscopy might be recommended if there are changes to the severity or frequency of symptoms or ...</t>
-  </si>
-  <si>
     <t>What is the pathophysiology behind hepatic encephalopathy in cirrhosis?</t>
   </si>
   <si>
     <t>It results from accumulation of neurotoxins (mainly ammonia) due to impaired hepatic detoxification and portosystemic shunting.</t>
   </si>
   <si>
-    <t>Based on the information I found:
-The treatment of hepatic encephalopathy. Metab Brain Dis. 2007;22:389-405. doi: 10.1007/s11011-007-9060-7. [Google Scholar] 24. Butterworth RF, Kircheis G, Hilger N, et al. Efficacy of l-ornithine l-aspartate for the treatment of hepatic encephalopathy in cirrhosis: systematic review and meta-analysis of randomized controlled trials.
-Cirrhosis is the 12 th leading cause of death in the United States (US), accounting for more than 36,000 deaths and having a death rate of 11.5 per 100,000 in 2013.1 Hepatic encephalopathy (HE) is one of the most debilitating complications of cirrhosis and severely affects the lives of patients and their caregivers.2 HE embodies a spectrum of ...</t>
-  </si>
-  <si>
     <t>What stool findings support a diagnosis of chronic pancreatitis?</t>
   </si>
   <si>
-    <t>Based on the information I found:
-Chronic pancreatitis is a permanent, progressive destruction of pancreatic tissue and function. Clinical manifestations include disabling abdominal pain, steatorrhea, and diabetes mellitus. 1 ...
-The fat in the stool makes the stool greasy or oily. Patients with chronic pancreatitis may also notice oil drops on the toilet water's surface. 3. Floating stools. The high-fat content of the stool in patients with chronic pancreatitis prevents the stool from being soaked in water. As a result, your stool maintains its low density and floats ..</t>
-  </si>
-  <si>
     <t>Steatorrhea (fatty, foul-smelling stools) due to exocrine insufficiency, confirmed by low fecal elastase levels.</t>
   </si>
   <si>
@@ -162,14 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Endoscopic surveillance every 3–5 years for non-dysplastic Barrett’s; more frequently if dysplasia is present.</t>
-  </si>
-  <si>
-    <t>Based on the information I found:
-surveillance in patients with Barrett's esophagus (BE) and is based on systematic reviews of the evidence using the Grading of Recommendations, Assessment, Develop-ment and Evaluation methodology. The document ad-dresses key clinical questions that include the role and impact of screening and surveillance and the utility of
-This document is the official American Society for Gastrointestinal Endoscopy guideline on screening and surveillance in patients with Barrett's esophagus (BE) and is based on systematic reviews of the evidence using the Grading of Recommendations, Assessment, Development and Evaluation methodology. The document addresses key clinical questions that include the role and impact of screening ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer from the search (App) </t>
   </si>
 </sst>
 </file>
@@ -579,20 +514,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D541741E-0F0F-4164-99D4-6E8DAD031701}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="58.5546875" customWidth="1"/>
     <col min="3" max="3" width="58.109375" customWidth="1"/>
-    <col min="4" max="4" width="61.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -602,11 +536,8 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -616,11 +547,8 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="388.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -630,241 +558,194 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="360" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="360" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>